<commit_message>
422 error with polygon search
</commit_message>
<xml_diff>
--- a/try.xlsx
+++ b/try.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\workspace\kfintech\RealEstateAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8254CBA-BDEB-4205-B72C-922CEEF43EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8174AD7-22CC-4738-A424-03A31E424A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="2832" windowWidth="19200" windowHeight="8520" xr2:uid="{F060D7B3-12F6-4DB7-86F4-078299BC4723}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F060D7B3-12F6-4DB7-86F4-078299BC4723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -456,7 +456,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,7 +489,7 @@
         <v>915000</v>
       </c>
       <c r="D2">
-        <v>259.2</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -503,7 +503,7 @@
         <v>480600</v>
       </c>
       <c r="D3">
-        <v>548.52</v>
+        <v>548</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -517,7 +517,7 @@
         <v>607230</v>
       </c>
       <c r="D4">
-        <v>134.94</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>